<commit_message>
Add Data Platform Lab updates
</commit_message>
<xml_diff>
--- a/Cost Estimate.xlsx
+++ b/Cost Estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\DSBA6190-Spring2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B582906C-6CC3-46CD-B2C8-AEE62262476C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4F0E0A-C8F5-4BC0-97E0-353919FDC9E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{C570FB7A-9022-41D3-89C6-30A3E2756A3C}"/>
   </bookViews>
@@ -112,12 +112,169 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -126,12 +283,29 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -451,7 +625,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,103 +634,111 @@
     <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>1472.75</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <f>B2*C2</f>
         <v>736.375</v>
       </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <f t="shared" ref="D3:D5" si="0">B3*C3</f>
         <v>80</v>
       </c>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>2836.4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>2836.4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <f>1582.64 + 4464</f>
         <v>6046.64</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <f t="shared" si="0"/>
         <v>6046.64</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="11">
         <f>SUM(D2:D5)</f>
         <v>9699.4150000000009</v>
       </c>
+      <c r="E6" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>